<commit_message>
The great refactoring part 1
</commit_message>
<xml_diff>
--- a/Data_files/Part_1/Graph_randstad.xlsx
+++ b/Data_files/Part_1/Graph_randstad.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\Part_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9859D0-0802-4116-87C1-77AEF4CF6151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17440EFE-1B02-4638-AF8F-D99D9279661F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,9 +59,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
-  <si>
-    <t>Cities</t>
-  </si>
   <si>
     <t>Population</t>
   </si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>Schiedam</t>
+  </si>
+  <si>
+    <t>Locations</t>
   </si>
 </sst>
 </file>
@@ -500,27 +500,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
       </c>
       <c r="F1">
         <v>0</v>
@@ -591,7 +589,7 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>111834</v>
@@ -675,7 +673,7 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>222825</v>
@@ -759,7 +757,7 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>114182</v>
@@ -843,7 +841,7 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>160759</v>
@@ -927,7 +925,7 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>918117</v>
@@ -1011,7 +1009,7 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>106086</v>
@@ -1095,7 +1093,7 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8">
         <v>562839</v>
@@ -1179,7 +1177,7 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>121434</v>
@@ -1263,7 +1261,7 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>75316</v>
@@ -1347,7 +1345,7 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>165396</v>
@@ -1431,7 +1429,7 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>93345</v>
@@ -1515,7 +1513,7 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>127089</v>
@@ -1599,7 +1597,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>663900</v>
@@ -1683,7 +1681,7 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15">
         <v>77999</v>
@@ -1767,7 +1765,7 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>162300</v>
@@ -1851,7 +1849,7 @@
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>72561</v>
@@ -1935,7 +1933,7 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>367947</v>
@@ -2019,7 +2017,7 @@
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>75079</v>
@@ -2103,7 +2101,7 @@
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>114887</v>
@@ -2187,7 +2185,7 @@
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>53244</v>
@@ -2271,7 +2269,7 @@
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>159618</v>
@@ -2355,7 +2353,7 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>126998</v>
@@ -2442,6 +2440,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000967D3B9FC1DD84EB00B55E5790AB85E" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="92ec66a21d0d7142cf1fb1ae8fa08641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6ba023f1-a19b-4eec-904c-052d1f1cb5e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62a86672aac255264bf3f3decc56659c" ns2:_="">
     <xsd:import namespace="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
@@ -2585,35 +2598,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A82C749-3C2A-47C7-ADA8-29A0588A6394}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DAC06B8-1F73-47DE-927D-2B7240518635}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2635,9 +2623,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DAC06B8-1F73-47DE-927D-2B7240518635}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A82C749-3C2A-47C7-ADA8-29A0588A6394}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
messed and the last one and fixed it here
</commit_message>
<xml_diff>
--- a/Data_files/Part_1/Graph_randstad.xlsx
+++ b/Data_files/Part_1/Graph_randstad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\Part_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72703FDC-6B90-4C4E-909B-EFB1B5197A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549DC3F0-8540-4000-8DBE-4B0F2AAD5C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -501,7 +501,7 @@
   <dimension ref="A1:AA23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Z32" sqref="Z32"/>
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1750,7 +1750,7 @@
         <v>0</v>
       </c>
       <c r="W15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X15" s="1">
         <v>0</v>
@@ -2073,7 +2073,7 @@
         <v>0</v>
       </c>
       <c r="S19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T19">
         <v>0</v>
@@ -2442,6 +2442,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000967D3B9FC1DD84EB00B55E5790AB85E" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="92ec66a21d0d7142cf1fb1ae8fa08641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6ba023f1-a19b-4eec-904c-052d1f1cb5e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62a86672aac255264bf3f3decc56659c" ns2:_="">
     <xsd:import namespace="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
@@ -2585,35 +2600,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A82C749-3C2A-47C7-ADA8-29A0588A6394}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DAC06B8-1F73-47DE-927D-2B7240518635}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2635,9 +2625,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DAC06B8-1F73-47DE-927D-2B7240518635}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A82C749-3C2A-47C7-ADA8-29A0588A6394}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
messed up still and fixed even more
</commit_message>
<xml_diff>
--- a/Data_files/Part_1/Graph_randstad.xlsx
+++ b/Data_files/Part_1/Graph_randstad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\Part_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549DC3F0-8540-4000-8DBE-4B0F2AAD5C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFD67FC-DA42-454A-B715-1DBF3B5D77C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -501,7 +501,7 @@
   <dimension ref="A1:AA23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+      <selection activeCell="X36" sqref="X36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1918,7 +1918,7 @@
         <v>0</v>
       </c>
       <c r="W17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X17" s="1">
         <v>0</v>
@@ -2079,7 +2079,7 @@
         <v>0</v>
       </c>
       <c r="U19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V19">
         <v>0</v>
@@ -2442,21 +2442,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000967D3B9FC1DD84EB00B55E5790AB85E" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="92ec66a21d0d7142cf1fb1ae8fa08641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6ba023f1-a19b-4eec-904c-052d1f1cb5e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62a86672aac255264bf3f3decc56659c" ns2:_="">
     <xsd:import namespace="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
@@ -2600,10 +2585,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DAC06B8-1F73-47DE-927D-2B7240518635}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A82C749-3C2A-47C7-ADA8-29A0588A6394}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2625,19 +2635,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A82C749-3C2A-47C7-ADA8-29A0588A6394}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DAC06B8-1F73-47DE-927D-2B7240518635}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>